<commit_message>
More work on JPADStaticWriteUtils.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/CS300/PERFORMANCE/XCG_0.25/Performance_0.25.xlsx
+++ b/JPADSandBox_v2/out/CS300/PERFORMANCE/XCG_0.25/Performance_0.25.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="101">
   <si>
     <t>Description</t>
   </si>
@@ -223,39 +223,6 @@
   </si>
   <si>
     <t>Landing duration</t>
-  </si>
-  <si>
-    <t>ALTITUDE</t>
-  </si>
-  <si>
-    <t>MACH</t>
-  </si>
-  <si>
-    <t>RANGE AT MAX PAYLOAD</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>Aircraft mass</t>
-  </si>
-  <si>
-    <t>Payload mass</t>
-  </si>
-  <si>
-    <t>Passengers number</t>
-  </si>
-  <si>
-    <t>Fuel mass</t>
-  </si>
-  <si>
-    <t>RANGE AT DESIGN PAYLOAD</t>
-  </si>
-  <si>
-    <t>RANGE AT MAX FUEL</t>
-  </si>
-  <si>
-    <t>RANGE AT ZERO PAYLOAD</t>
   </si>
   <si>
     <t>REGULATION</t>
@@ -1603,301 +1570,8 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="35"/>
-  <cols>
-    <col min="2" max="2" width="8.0" customWidth="true"/>
-    <col min="3" max="3" width="15.0" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="n">
-        <v>36999.99999999999</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="n">
-        <v>67585.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" t="n">
-        <v>16800.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="n">
-        <v>160.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="n">
-        <v>13703.999999999996</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="n">
-        <v>67585.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="n">
-        <v>15750.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" t="n">
-        <v>150.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="n">
-        <v>14753.999999999995</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" t="n">
-        <v>67585.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" t="n">
-        <v>10503.999999999996</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" t="n">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" t="n">
-        <v>20000.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" t="n">
-        <v>57080.999999999985</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" t="n">
-        <v>20000.0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -1927,24 +1601,24 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4">
@@ -1959,12 +1633,12 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -1975,7 +1649,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1986,7 +1660,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1997,7 +1671,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
@@ -2008,12 +1682,12 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -2024,7 +1698,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
@@ -2035,7 +1709,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -2046,12 +1720,12 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
@@ -2062,7 +1736,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -2073,7 +1747,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
@@ -2084,12 +1758,12 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
@@ -2100,7 +1774,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -2111,7 +1785,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -2122,12 +1796,12 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
@@ -2138,7 +1812,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
         <v>19</v>
@@ -2149,7 +1823,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
@@ -2160,12 +1834,12 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
@@ -2176,7 +1850,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
         <v>19</v>
@@ -2187,7 +1861,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
         <v>21</v>
@@ -2198,12 +1872,12 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
         <v>13</v>
@@ -2214,7 +1888,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
         <v>19</v>
@@ -2225,7 +1899,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
         <v>21</v>
@@ -2241,17 +1915,17 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
         <v>13</v>
@@ -2262,7 +1936,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
         <v>19</v>
@@ -2273,7 +1947,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
         <v>21</v>
@@ -2284,12 +1958,12 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
         <v>13</v>
@@ -2300,7 +1974,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
         <v>19</v>
@@ -2311,7 +1985,7 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
         <v>21</v>
@@ -2322,12 +1996,12 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B46" t="s">
         <v>13</v>
@@ -2338,7 +2012,7 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B47" t="s">
         <v>19</v>
@@ -2349,7 +2023,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B48" t="s">
         <v>21</v>
@@ -2360,12 +2034,12 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
@@ -2376,7 +2050,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B51" t="s">
         <v>19</v>
@@ -2387,7 +2061,7 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
         <v>21</v>
@@ -2398,12 +2072,12 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
         <v>13</v>
@@ -2414,7 +2088,7 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
         <v>19</v>
@@ -2425,7 +2099,7 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B56" t="s">
         <v>21</v>
@@ -2436,12 +2110,12 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B58" t="s">
         <v>13</v>
@@ -2452,7 +2126,7 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B59" t="s">
         <v>19</v>
@@ -2463,7 +2137,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B60" t="s">
         <v>21</v>
@@ -2484,12 +2158,12 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B64" t="s">
         <v>13</v>
@@ -2500,7 +2174,7 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B65" t="s">
         <v>19</v>
@@ -2511,12 +2185,12 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B67" t="s">
         <v>13</v>
@@ -2527,7 +2201,7 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B68" t="s">
         <v>19</v>
@@ -2538,7 +2212,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B69" t="s">
         <v>21</v>
@@ -2549,12 +2223,12 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
         <v>13</v>
@@ -2565,7 +2239,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B72" t="s">
         <v>19</v>
@@ -2576,7 +2250,7 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B73" t="s">
         <v>21</v>
@@ -2592,17 +2266,17 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B77" t="s">
         <v>13</v>
@@ -2613,7 +2287,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B78" t="s">
         <v>19</v>
@@ -2624,7 +2298,7 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
         <v>21</v>
@@ -2635,12 +2309,12 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B81" t="s">
         <v>13</v>
@@ -2651,7 +2325,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B82" t="s">
         <v>19</v>
@@ -2662,7 +2336,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B83" t="s">
         <v>21</v>

</xml_diff>